<commit_message>
enforces storage capacity deployment
Former-commit-id: ae4dfe33d4abe2747489610f1b4b5072b5f6b9ac
Former-commit-id: 1ab329bb4ed454b1fd9d21ff46d6c4ecec321a5e
</commit_message>
<xml_diff>
--- a/data/timeslices_solar_wind_cf.xlsx
+++ b/data/timeslices_solar_wind_cf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1CFC31-B12D-4A2E-B048-569750596FA0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1370AB61-BB98-4D14-97AB-476860EE5436}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A566AB5E-42BF-4D57-AEBC-9280CA97FF98}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A3:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C11"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>